<commit_message>
base and build trip tables instead of alt
</commit_message>
<xml_diff>
--- a/bca4abm/tests/data/bca4abm-sample-data.xlsx
+++ b/bca4abm/tests/data/bca4abm-sample-data.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="5100" windowWidth="39960" windowHeight="21660" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="3120" yWindow="3680" windowWidth="39960" windowHeight="21660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="households" sheetId="1" r:id="rId1"/>
-    <sheet name="persons" sheetId="2" r:id="rId2"/>
+    <sheet name="persons.csv" sheetId="2" r:id="rId2"/>
     <sheet name="basetrips" sheetId="3" r:id="rId3"/>
     <sheet name="basetrips_alt" sheetId="4" r:id="rId4"/>
     <sheet name="buildtrips" sheetId="5" r:id="rId5"/>
@@ -2396,10 +2396,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3297,36 +3297,6 @@
         <v>2</v>
       </c>
       <c r="J28" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>100</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3</v>
-      </c>
-      <c r="D29" s="1">
-        <v>78</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2</v>
-      </c>
-      <c r="F29" s="1">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1">
-        <v>1</v>
-      </c>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1">
         <v>0</v>
       </c>
     </row>
@@ -21044,7 +21014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>